<commit_message>
ECP-1197: adds date signed to import / export; also now defaults to date of upload instead of leaving the field empty
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/lease_amendment_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/lease_amendment_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1901A92A-0C53-9A41-B3E1-95ECA9CB42A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363BE0C4-93B4-E84A-9522-4DA8A40B7FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
   <si>
     <t>Lease Amendment Type</t>
   </si>
@@ -104,6 +104,9 @@
   </si>
   <si>
     <t>APPLY</t>
+  </si>
+  <si>
+    <t>Date Signed</t>
   </si>
 </sst>
 </file>
@@ -477,34 +480,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="37" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,62 +516,67 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1">
+        <v>44004</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="1">
+      <c r="E2" s="1">
         <v>44013</v>
       </c>
-      <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -579,130 +588,136 @@
       <c r="N2" s="2"/>
       <c r="O2" s="2"/>
       <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="1">
+      <c r="E3" s="1">
         <v>44013</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2">
         <v>55.55</v>
       </c>
-      <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="2"/>
+      <c r="J3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>44013</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>44074</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="1">
+      <c r="P3" s="1">
         <v>44013</v>
       </c>
-      <c r="P3" s="1">
+      <c r="Q3" s="1">
         <v>44196</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1">
+        <v>44002</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>44013</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2">
+      <c r="F4" s="2"/>
+      <c r="G4" s="2">
         <v>100</v>
       </c>
-      <c r="G4" s="2"/>
       <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <v>44013</v>
       </c>
-      <c r="K4" s="1">
+      <c r="L4" s="1">
         <v>44074</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="1">
+      <c r="P4" s="1">
         <v>44013</v>
       </c>
-      <c r="P4" s="1">
+      <c r="Q4" s="1">
         <v>44196</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>43983</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2">
+      <c r="F5" s="2"/>
+      <c r="G5" s="2">
         <v>100</v>
       </c>
-      <c r="G5" s="3">
+      <c r="H5" s="3">
         <v>-3500.12</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>44014</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>44073</v>
       </c>
-      <c r="L5" s="2"/>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="1"/>
+      <c r="O5" s="2"/>
       <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
ECP-1224: adds support for multiple amendment items for discount
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/lease_amendment_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/lease_amendment_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363BE0C4-93B4-E84A-9522-4DA8A40B7FB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B23303F-50F7-BB40-94D1-4608ECB88C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
     <t>Lease Amendment Type</t>
   </si>
@@ -480,11 +480,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -687,31 +687,31 @@
         <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="C5" s="1">
+        <v>44002</v>
+      </c>
       <c r="D5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E5" s="1">
-        <v>43983</v>
+        <v>44013</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2">
-        <v>100</v>
-      </c>
-      <c r="H5" s="3">
-        <v>-3500.12</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="K5" s="1">
-        <v>44014</v>
+        <v>44075</v>
       </c>
       <c r="L5" s="1">
-        <v>44073</v>
+        <v>44104</v>
       </c>
       <c r="M5" s="2"/>
       <c r="N5" s="2"/>
@@ -719,6 +719,70 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1">
+        <v>44002</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="1">
+        <v>44013</v>
+      </c>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2">
+        <v>25</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K6" s="1">
+        <v>44105</v>
+      </c>
+      <c r="L6" s="1">
+        <v>44135</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1">
+        <v>43983</v>
+      </c>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>100</v>
+      </c>
+      <c r="H7" s="3">
+        <v>-3500.12</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K7" s="1">
+        <v>44014</v>
+      </c>
+      <c r="L7" s="1">
+        <v>44073</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ECP-1282: renames lease amendment type to lease amendment template
</commit_message>
<xml_diff>
--- a/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/lease_amendment_import.xlsx
+++ b/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/lease_amendment_import.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johan/src/estatio-ecp/estatio/estatioapp/app/src/main/java/org/estatio/module/lease/fixtures/imports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B23303F-50F7-BB40-94D1-4608ECB88C32}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316D9044-7E92-4A45-B478-9973FC996791}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="21940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="29">
   <si>
-    <t>Lease Amendment Type</t>
-  </si>
-  <si>
     <t>Lease Amendment State</t>
   </si>
   <si>
@@ -107,6 +104,9 @@
   </si>
   <si>
     <t>Date Signed</t>
+  </si>
+  <si>
+    <t>Lease Amendment Template</t>
   </si>
 </sst>
 </file>
@@ -484,12 +484,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
     <col min="4" max="4" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -510,69 +510,69 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C2" s="1">
         <v>44004</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1">
         <v>44013</v>
@@ -592,14 +592,14 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>16</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="1">
         <v>44013</v>
@@ -611,7 +611,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="1">
         <v>44013</v>
@@ -620,13 +620,13 @@
         <v>44074</v>
       </c>
       <c r="M3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="P3" s="1">
         <v>44013</v>
@@ -637,16 +637,16 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="1">
         <v>44002</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1">
         <v>44013</v>
@@ -658,7 +658,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K4" s="1">
         <v>44013</v>
@@ -667,13 +667,13 @@
         <v>44074</v>
       </c>
       <c r="M4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="P4" s="1">
         <v>44013</v>
@@ -684,16 +684,16 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1">
         <v>44002</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1">
         <v>44013</v>
@@ -705,7 +705,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K5" s="1">
         <v>44075</v>
@@ -721,16 +721,16 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="1">
         <v>44002</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E6" s="1">
         <v>44013</v>
@@ -742,7 +742,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K6" s="1">
         <v>44105</v>
@@ -753,14 +753,14 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E7" s="1">
         <v>43983</v>
@@ -774,7 +774,7 @@
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K7" s="1">
         <v>44014</v>

</xml_diff>